<commit_message>
마지막 라인 merge check
</commit_message>
<xml_diff>
--- a/lecture.xlsx
+++ b/lecture.xlsx
@@ -4270,6 +4270,11 @@
       </c>
     </row>
     <row r="178">
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>ch02. AWS EMR에 배포</t>
+        </is>
+      </c>
       <c r="C178" t="inlineStr">
         <is>
           <t>CH02_01. AWS EMR에서 Spark application 실행</t>
@@ -4286,7 +4291,6 @@
     <mergeCell ref="A8:A30"/>
     <mergeCell ref="B161:B169"/>
     <mergeCell ref="B127"/>
-    <mergeCell ref="B172:B178"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="B64:B71"/>
     <mergeCell ref="B30"/>
@@ -4320,6 +4324,7 @@
     <mergeCell ref="B10:B15"/>
     <mergeCell ref="B128:B142"/>
     <mergeCell ref="B42"/>
+    <mergeCell ref="B172:B177"/>
     <mergeCell ref="B72:B78"/>
     <mergeCell ref="A112:A159"/>
     <mergeCell ref="B54:B55"/>
@@ -11760,6 +11765,11 @@
       </c>
     </row>
     <row r="468">
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Ch 05. 모의 시험 문제 풀이</t>
+        </is>
+      </c>
       <c r="C468" t="inlineStr">
         <is>
           <t>01.모의 시험 문제 풀이</t>
@@ -11776,7 +11786,6 @@
     <mergeCell ref="B385:B388"/>
     <mergeCell ref="B137:B141"/>
     <mergeCell ref="B311:B316"/>
-    <mergeCell ref="B462:B468"/>
     <mergeCell ref="A422:A438"/>
     <mergeCell ref="B58:B67"/>
     <mergeCell ref="B295:B299"/>
@@ -11830,6 +11839,7 @@
     <mergeCell ref="B382:B384"/>
     <mergeCell ref="B97:B103"/>
     <mergeCell ref="B362"/>
+    <mergeCell ref="B462:B467"/>
     <mergeCell ref="B352:B354"/>
     <mergeCell ref="A311:A351"/>
     <mergeCell ref="B132:B136"/>
@@ -23622,6 +23632,11 @@
       </c>
     </row>
     <row r="231">
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Chapter.05 Advanced Topic</t>
+        </is>
+      </c>
       <c r="C231" t="inlineStr">
         <is>
           <t>CH05_01 못다한 이야기들</t>
@@ -23645,6 +23660,7 @@
     <mergeCell ref="B220:B221"/>
     <mergeCell ref="B172:B180"/>
     <mergeCell ref="A185:A213"/>
+    <mergeCell ref="B229:B230"/>
     <mergeCell ref="B48:B58"/>
     <mergeCell ref="B157:B171"/>
     <mergeCell ref="B96:B116"/>
@@ -23661,7 +23677,6 @@
     <mergeCell ref="B76:B95"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B145:B156"/>
-    <mergeCell ref="B229:B231"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="B212:B213"/>
     <mergeCell ref="B21:B25"/>

</xml_diff>